<commit_message>
Add APIs and dashboards for inventory and shipments
Added new API endpoints for shipment planning and engineering routes, as well as dashboards for inventory management. Updated database configuration for remote connection. Introduced new process and dashboard PHP files to support inventory, manufacturing, QA, and replenishment workflows.
</commit_message>
<xml_diff>
--- a/public/sql/Estructura_Cardex.xlsx
+++ b/public/sql/Estructura_Cardex.xlsx
@@ -22958,4 +22958,286 @@
   <pageSetup paperSize="32767" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101000B542A4FC3E1184F94A61D515BBBD255" ma:contentTypeVersion="17" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="b5cc52f47dc9b6b3b27cb3f2445b51da">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="dcdd6b4c-2297-40ec-823b-44e6acde9918" xmlns:ns3="ddc5e77b-0712-4e63-afd1-70859558c0b6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="319243247cf4cca3c33d3dfd77803bcc" ns2:_="" ns3:_="">
+    <xsd:import namespace="dcdd6b4c-2297-40ec-823b-44e6acde9918"/>
+    <xsd:import namespace="ddc5e77b-0712-4e63-afd1-70859558c0b6"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:API" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="dcdd6b4c-2297-40ec-823b-44e6acde9918" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="11" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="12" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="13" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="14" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="17" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="18" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="20" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Etiquetas de imagen" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="eb1238be-2ba0-423a-86e6-e9a5321a64e5" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="22" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="23" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="API" ma:index="24" nillable="true" ma:displayName="API" ma:default="API Voice Picking" ma:description="Aplicación" ma:format="Dropdown" ma:internalName="API">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="ddc5e77b-0712-4e63-afd1-70859558c0b6" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="15" nillable="true" ma:displayName="Compartido con" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="16" nillable="true" ma:displayName="Detalles de uso compartido" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="21" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{6b414cfa-d0cd-459a-8d3c-e9b45a13284e}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="ddc5e77b-0712-4e63-afd1-70859558c0b6">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de contenido"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="dcdd6b4c-2297-40ec-823b-44e6acde9918">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="ddc5e77b-0712-4e63-afd1-70859558c0b6" xsi:nil="true"/>
+    <API xmlns="dcdd6b4c-2297-40ec-823b-44e6acde9918">API Voice Picking</API>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{227D3719-160E-432B-93E0-A9211B98EDB9}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D18C810D-5049-4CB7-BEE6-2C76E2143DBB}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83F811C4-454E-4536-BAC7-2F95BF995F32}"/>
 </file>
</xml_diff>